<commit_message>
continued with map and bgt
</commit_message>
<xml_diff>
--- a/data-raw/bgt_names_features.xlsx
+++ b/data-raw/bgt_names_features.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KNMI\Dropbox\KNMI\R_SPQJ\wmoSC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3889464F-D4CC-4496-8E55-E707FB510358}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A500DDA4-3E65-4A85-947E-AE6A3D00AF54}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{5178EE40-75D6-42FB-8636-77CC4C46320D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="2" xr2:uid="{5178EE40-75D6-42FB-8636-77CC4C46320D}"/>
   </bookViews>
   <sheets>
     <sheet name="bgt_objects" sheetId="1" r:id="rId1"/>
-    <sheet name="bgt_features_perObject" sheetId="2" r:id="rId2"/>
+    <sheet name="object_fields" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="bgt_features_perObject" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>begroeidterreindeel</t>
   </si>
@@ -236,6 +238,24 @@
   </si>
   <si>
     <t>kering</t>
+  </si>
+  <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>gml_id</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -279,9 +299,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +622,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,10 +727,192 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72A9136-8DA9-4210-9EF4-D48AD2A2192F}">
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C0DBAE-B30B-48EC-B0F0-9AD7FCEA5081}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>140803</v>
+      </c>
+      <c r="C2">
+        <v>456882</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D393605D-FF07-41F8-989B-0799FDC4C358}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
preprocess and process bgt
</commit_message>
<xml_diff>
--- a/data-raw/bgt_names_features.xlsx
+++ b/data-raw/bgt_names_features.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bgt_objects" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="133">
   <si>
     <t xml:space="preserve">object_short_name</t>
   </si>
@@ -147,6 +147,9 @@
     <t xml:space="preserve">lokaalid</t>
   </si>
   <si>
+    <t xml:space="preserve">object</t>
+  </si>
+  <si>
     <t xml:space="preserve">plus-sta_2</t>
   </si>
   <si>
@@ -196,6 +199,9 @@
   </si>
   <si>
     <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">plus.statu</t>
@@ -559,7 +565,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="Y74:AB76 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -676,8 +682,8 @@
   </sheetPr>
   <dimension ref="A1:AJ114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O59" activeCellId="0" sqref="O59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB74" activeCellId="0" sqref="Y74:AB76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -713,7 +719,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="8"/>
@@ -1302,7 +1308,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>31</v>
       </c>
@@ -1336,6 +1342,9 @@
       <c r="N8" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="P8" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="Q8" s="0" t="s">
         <v>20</v>
       </c>
@@ -1346,7 +1355,7 @@
         <v>26</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V8" s="0" t="s">
         <v>38</v>
@@ -1355,7 +1364,7 @@
         <v>26</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Z8" s="0" t="s">
         <v>38</v>
@@ -1384,19 +1393,19 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>30</v>
@@ -1414,7 +1423,7 @@
         <v>34</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q9" s="0" t="s">
         <v>25</v>
@@ -1426,7 +1435,7 @@
         <v>31</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V9" s="0" t="s">
         <v>40</v>
@@ -1435,7 +1444,7 @@
         <v>31</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Z9" s="0" t="s">
         <v>40</v>
@@ -1447,13 +1456,13 @@
         <v>37</v>
       </c>
       <c r="AD9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AF9" s="0" t="s">
         <v>35</v>
       </c>
       <c r="AG9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH9" s="0" t="s">
         <v>38</v>
@@ -1464,19 +1473,19 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>35</v>
@@ -1485,7 +1494,7 @@
         <v>30</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>35</v>
@@ -1494,7 +1503,7 @@
         <v>37</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q10" s="0" t="s">
         <v>30</v>
@@ -1506,28 +1515,28 @@
         <v>35</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AF10" s="5" t="s">
         <v>39</v>
       </c>
       <c r="AG10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AH10" s="0" t="s">
         <v>40</v>
@@ -1536,12 +1545,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>39</v>
@@ -1550,43 +1559,43 @@
         <v>26</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AB11" s="5" t="s">
         <v>25</v>
@@ -1595,69 +1604,84 @@
         <v>28</v>
       </c>
       <c r="AD11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="AF11" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="AG11" s="0" t="s">
         <v>35</v>
       </c>
       <c r="AH11" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ11" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="M12" s="0" t="s">
         <v>28</v>
       </c>
       <c r="N12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="V12" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="Q12" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="R12" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="V12" s="0" t="s">
-        <v>50</v>
       </c>
       <c r="X12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AB12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="AC12" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AD12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AH12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AJ12" s="5" t="s">
         <v>39</v>
@@ -1665,31 +1689,31 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="M13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="V13" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="N13" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="R13" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="V13" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="X13" s="0" t="s">
         <v>35</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AB13" s="0" t="s">
         <v>35</v>
@@ -1698,56 +1722,59 @@
         <v>33</v>
       </c>
       <c r="AD13" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AH13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="AJ13" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M14" s="0" t="s">
         <v>33</v>
       </c>
       <c r="N14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="V14" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="R14" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="V14" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="X14" s="5" t="s">
         <v>39</v>
       </c>
       <c r="Z14" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AB14" s="5" t="s">
         <v>39</v>
       </c>
       <c r="AD14" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AH14" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="F15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>36</v>
@@ -1756,30 +1783,36 @@
         <v>26</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="Z15" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="AB15" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="AH15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M16" s="0" t="s">
         <v>31</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AH16" s="0" t="s">
         <v>20</v>
@@ -1787,13 +1820,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AH17" s="0" t="s">
         <v>25</v>
@@ -1801,59 +1834,59 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="AH18" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N19" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="n">
         <f aca="false">COUNTA(A3:A20)+COUNTA(D3:D20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H21" s="0" t="n">
         <f aca="false">COUNTA(E3:E20)+COUNTA(H3:H20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L21" s="0" t="n">
         <f aca="false">COUNTA(I3:I20)+COUNTA(L3:L20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">COUNTA(M3:M20)+COUNTA(P3:P20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T21" s="0" t="n">
         <f aca="false">COUNTA(Q3:Q20)+COUNTA(T3:T20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="X21" s="0" t="n">
         <f aca="false">COUNTA(U3:U20)+COUNTA(X3:X20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AB21" s="0" t="n">
         <f aca="false">COUNTA(Y3:Y20)+COUNTA(AB3:AB20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AF21" s="0" t="n">
         <f aca="false">COUNTA(AC3:AC20)+COUNTA(AF3:AF20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AJ21" s="0" t="n">
         <f aca="false">COUNTA(AG3:AG20)+COUNTA(AJ3:AJ20)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,7 +1934,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>22</v>
@@ -1909,13 +1942,13 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>19</v>
@@ -1998,7 +2031,7 @@
         <v>9</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2018,7 +2051,7 @@
         <v>9</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,7 +2076,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">COUNTIF(A$3:A$20,A35)+COUNTIF(E$3:E$20,A35)+COUNTIF(I$3:I$20,A35)+COUNTIF(M$3:M$20,A35)+COUNTIF(Q$3:Q$20,A35)+COUNTIF(U$3:U$20,A35)+COUNTIF(Y$3:Y$20,A35)+COUNTIF(AC$3:AC$20,A35)+COUNTIF(AG$3:AG$20,A35)</f>
@@ -2063,7 +2096,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">COUNTIF(A$3:A$20,A36)+COUNTIF(E$3:E$20,A36)+COUNTIF(I$3:I$20,A36)+COUNTIF(M$3:M$20,A36)+COUNTIF(Q$3:Q$20,A36)+COUNTIF(U$3:U$20,A36)+COUNTIF(Y$3:Y$20,A36)+COUNTIF(AC$3:AC$20,A36)+COUNTIF(AG$3:AG$20,A36)</f>
@@ -2178,7 +2211,7 @@
         <v>9</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2198,7 +2231,7 @@
         <v>9</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,7 +2314,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
         <v>39</v>
       </c>
@@ -2301,17 +2334,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <f aca="false">COUNTA(A29:A47)</f>
-        <v>19</v>
-      </c>
-      <c r="C48" s="4"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <f aca="false">COUNTIF(A$3:A$20,A48)+COUNTIF(E$3:E$20,A48)+COUNTIF(I$3:I$20,A48)+COUNTIF(M$3:M$20,A48)+COUNTIF(Q$3:Q$20,A48)+COUNTIF(U$3:U$20,A48)+COUNTIF(Y$3:Y$20,A48)+COUNTIF(AC$3:AC$20,A48)+COUNTIF(AG$3:AG$20,A48)</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="4" t="n">
+        <f aca="false">COUNTIF(D$3:D$20,A48)+COUNTIF(H$3:H$20,A48)+COUNTIF(L$3:L$20,A48)+COUNTIF(P$3:P$20,A48)+COUNTIF(T$3:T$20,A48)+COUNTIF(X$3:X$20,A48)+COUNTIF(AB$3:AB$20,A48)+COUNTIF(AF$3:AF$20,A48)+COUNTIF(AJ$3:AJ$20,A48)</f>
+        <v>9</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <f aca="false">SUM(B48:C48)</f>
+        <v>9</v>
+      </c>
       <c r="H48" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <f aca="false">COUNTA(A29:A48)</f>
+        <v>20</v>
+      </c>
       <c r="C49" s="4"/>
       <c r="H49" s="0" t="s">
         <v>20</v>
@@ -2327,30 +2374,36 @@
       <c r="A51" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B51" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="C51" s="4"/>
       <c r="H51" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>39</v>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C52" s="4"/>
       <c r="H52" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L52" s="0" t="s">
         <v>15</v>
       </c>
       <c r="M52" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N52" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="O52" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P52" s="0" t="s">
         <v>34</v>
@@ -2359,63 +2412,72 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C53" s="4"/>
       <c r="H53" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L53" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M53" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N53" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O53" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="P53" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q53" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C54" s="4"/>
       <c r="H54" s="0" t="s">
         <v>15</v>
       </c>
       <c r="L54" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M54" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N54" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="O54" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P54" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q54" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>67</v>
+        <v>35</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C55" s="4"/>
       <c r="H55" s="0" t="s">
@@ -2425,18 +2487,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C56" s="4"/>
       <c r="H56" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C57" s="4"/>
       <c r="H57" s="0" t="s">
@@ -2446,24 +2514,27 @@
         <v>15</v>
       </c>
       <c r="M57" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N57" s="0" t="s">
         <v>18</v>
       </c>
       <c r="O57" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P57" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Q57" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C58" s="4"/>
       <c r="H58" s="0" t="s">
@@ -2473,58 +2544,64 @@
         <v>37</v>
       </c>
       <c r="M58" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N58" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O58" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P58" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q58" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C59" s="4"/>
       <c r="H59" s="0" t="s">
         <v>24</v>
       </c>
       <c r="L59" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="M59" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N59" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="O59" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="P59" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q59" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="M59" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="N59" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="O59" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="P59" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q59" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C60" s="4"/>
       <c r="H60" s="0" t="s">
         <v>34</v>
       </c>
       <c r="L60" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M60" s="0" t="s">
         <v>35</v>
@@ -2533,21 +2610,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>61</v>
+        <v>66</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C61" s="4"/>
       <c r="H61" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="0" t="s">
         <v>59</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L62" s="0" t="n">
         <f aca="false">COUNTIF($L$52:$Q$60,L52)</f>
@@ -2574,9 +2657,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="H63" s="0" t="s">
         <v>28</v>
@@ -2606,12 +2692,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
         <v>62</v>
       </c>
+      <c r="B64" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="H64" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L64" s="0" t="n">
         <f aca="false">COUNTIF($L$52:$Q$60,L54)</f>
@@ -2638,9 +2727,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="H65" s="0" t="s">
         <v>33</v>
@@ -2650,42 +2742,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="H66" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H67" s="0" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="H68" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="H69" s="0" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="H70" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="L70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H71" s="0" t="s">
@@ -2694,8 +2800,8 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7" t="str">
-        <f aca="false">_xlfn.CONCAT("c('"&amp;A51&amp;$A$27&amp;A52&amp;$A$27&amp;A53&amp;$A$27&amp;A54&amp;$A$27&amp;A55&amp;$A$27&amp;A56&amp;$A$27&amp;A53&amp;$A$27&amp;A58&amp;$A$27&amp;A59&amp;$A$27&amp;A60&amp;$A$27&amp;A61&amp;$A$27&amp;A62&amp;$A$27&amp;A63&amp;$A$27&amp;A64&amp;$A$27&amp;A65&amp;$A$27&amp;A66&amp;$A$27&amp;A67&amp;$A$27&amp;A68&amp;$A$27&amp;A69&amp;"')")</f>
-        <v>c('gml_id', 'object_typ', 'bronhouder', 'naam', 'bgt.functi', 'bgt.fysiek', 'bronhouder', 'plus.fun_1', 'plus.fun_2', 'plus.funct', 'plus.fys_2', 'plus.fysie', 'plus.sta_1', 'plus.sta_2', 'plus.statu', 'plus.typ_1', 'plus.type', 'relatieveh', 'status')</v>
+        <f aca="false">_xlfn.CONCAT("c('"&amp;A51&amp;$A$27&amp;A52&amp;$A$27&amp;$A53&amp;$A$27&amp;A54&amp;$A$27&amp;A55&amp;$A$27&amp;A56&amp;$A$27&amp;A57&amp;$A$27&amp;A54&amp;$A$27&amp;A59&amp;$A$27&amp;A60&amp;$A$27&amp;A61&amp;$A$27&amp;A62&amp;$A$27&amp;A63&amp;$A$27&amp;A64&amp;$A$27&amp;A65&amp;$A$27&amp;A66&amp;$A$27&amp;A67&amp;$A$27&amp;A68&amp;$A$27&amp;A69&amp;$A$27&amp;A70&amp;"')")</f>
+        <v>c('gml_id', 'object', 'object_typ', 'bronhouder', 'naam', 'bgt.functi', 'bgt.fysiek', 'bronhouder', 'plus.fun_1', 'plus.fun_2', 'plus.funct', 'plus.fys_2', 'plus.fysie', 'plus.sta_1', 'plus.sta_2', 'plus.statu', 'plus.typ_1', 'plus.type', 'relatieveh', 'status')</v>
       </c>
       <c r="H72" s="0" t="s">
         <v>37</v>
@@ -2718,12 +2824,12 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H76" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H77" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,12 +2859,12 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H83" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H84" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,12 +2894,12 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H90" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H91" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,7 +2939,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H99" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2843,7 +2949,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H101" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,12 +2989,12 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H109" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H110" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,8 +3032,8 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="1" sqref="Y74:AB76 G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2984,231 +3090,231 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>